<commit_message>
updated dashboard features & modified greco notebook
</commit_message>
<xml_diff>
--- a/data/processed/dim_patient_status.xlsx
+++ b/data/processed/dim_patient_status.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://musigma-my.sharepoint.com/personal/vignesh_nehru_mu-sigma_com/Documents/Documents/walmart/re_greco/data/processed/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F3280038C431921FD2FE31D2F87AC3C1615B219D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D441912C-D64C-48B2-AB01-129DB23E4627}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,11 +61,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,21 +129,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +173,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -221,7 +207,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -256,10 +241,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,21 +416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -483,7 +460,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -503,7 +480,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -523,7 +500,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -543,7 +520,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1001</v>
       </c>
@@ -563,7 +540,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>1001</v>
       </c>
@@ -583,7 +560,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1001</v>
       </c>
@@ -603,7 +580,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1002</v>
       </c>
@@ -620,7 +597,7 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1002</v>
       </c>
@@ -640,7 +617,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1002</v>
       </c>
@@ -660,7 +637,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1002</v>
       </c>
@@ -680,7 +657,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>1002</v>
       </c>
@@ -700,7 +677,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>1003</v>
       </c>
@@ -717,7 +694,7 @@
         <v>44630</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1003</v>
       </c>
@@ -737,7 +714,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>1003</v>
       </c>
@@ -757,7 +734,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>1004</v>
       </c>
@@ -774,7 +751,7 @@
         <v>42370</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>1004</v>
       </c>
@@ -794,7 +771,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>1005</v>
       </c>
@@ -811,7 +788,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>1005</v>
       </c>
@@ -831,7 +808,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>1005</v>
       </c>
@@ -851,7 +828,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>1006</v>
       </c>
@@ -868,7 +845,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>1007</v>
       </c>
@@ -885,7 +862,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>1007</v>
       </c>
@@ -905,7 +882,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>1007</v>
       </c>
@@ -925,7 +902,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>1007</v>
       </c>
@@ -945,7 +922,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>1008</v>
       </c>
@@ -962,7 +939,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>1008</v>
       </c>

</xml_diff>

<commit_message>
Created greco3 with updated logic regarding the add_status_and_recent_status function
</commit_message>
<xml_diff>
--- a/data/processed/dim_patient_status.xlsx
+++ b/data/processed/dim_patient_status.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://musigma-my.sharepoint.com/personal/vignesh_nehru_mu-sigma_com/Documents/Documents/walmart/re_greco/data/processed/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_B22E0038C431921FD2FE31D2F87AC3C1915765C5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4592FBCA-D277-4ECE-83B0-F7C46B5E3087}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -61,11 +67,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +135,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +187,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -207,6 +221,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -241,9 +256,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -416,14 +432,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -460,7 +483,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -480,7 +503,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -500,7 +523,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -520,7 +543,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1001</v>
       </c>
@@ -540,7 +563,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1001</v>
       </c>
@@ -560,7 +583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1001</v>
       </c>
@@ -580,7 +603,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1002</v>
       </c>
@@ -597,7 +620,7 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1002</v>
       </c>
@@ -617,7 +640,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1002</v>
       </c>
@@ -637,7 +660,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1002</v>
       </c>
@@ -657,7 +680,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1002</v>
       </c>
@@ -677,7 +700,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1003</v>
       </c>
@@ -694,7 +717,7 @@
         <v>44630</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1003</v>
       </c>
@@ -714,7 +737,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1003</v>
       </c>
@@ -734,7 +757,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1004</v>
       </c>
@@ -751,7 +774,7 @@
         <v>42370</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1004</v>
       </c>
@@ -771,7 +794,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1005</v>
       </c>
@@ -788,7 +811,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1005</v>
       </c>
@@ -808,7 +831,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1005</v>
       </c>
@@ -828,7 +851,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1006</v>
       </c>
@@ -845,7 +868,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1007</v>
       </c>
@@ -862,7 +885,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1007</v>
       </c>
@@ -882,7 +905,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1007</v>
       </c>
@@ -902,7 +925,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1007</v>
       </c>
@@ -922,7 +945,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1008</v>
       </c>
@@ -939,7 +962,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1008</v>
       </c>

</xml_diff>